<commit_message>
Training and test comparison of poly with lasso
</commit_message>
<xml_diff>
--- a/1_Algorithmic Toolbox/Puzzle.xlsx
+++ b/1_Algorithmic Toolbox/Puzzle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\1_Algorithmic Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8D8C58-8EDD-4405-9787-FF04F42DECBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B4FAA5-0BDA-41B3-AD8C-A7A79D5C0918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A81258F2-4D04-4C55-B3D0-F30CD1DCD642}"/>
   </bookViews>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A422C11-5B61-45BD-906C-B2B8A0B17EEF}">
-  <dimension ref="A2:AL9"/>
+  <dimension ref="A2:AL90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G50" sqref="G11:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -991,6 +991,966 @@
         <v>22</v>
       </c>
     </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>89</v>
+      </c>
+      <c r="I11">
+        <f>G11+H11</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>88</v>
+      </c>
+      <c r="I12">
+        <f>G12+H12</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>87</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:I24" si="2">G13+H13</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>86</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>85</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>84</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>83</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>82</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>81</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>80</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>79</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>78</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23">
+        <v>77</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>76</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <v>75</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ref="I25:I36" si="3">G25+H25</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>74</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>26</v>
+      </c>
+      <c r="H27">
+        <v>73</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>27</v>
+      </c>
+      <c r="H28">
+        <v>72</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>71</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>29</v>
+      </c>
+      <c r="H30">
+        <v>70</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>69</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>31</v>
+      </c>
+      <c r="H32">
+        <v>68</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33">
+        <v>67</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>33</v>
+      </c>
+      <c r="H34">
+        <v>66</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>34</v>
+      </c>
+      <c r="H35">
+        <v>65</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>35</v>
+      </c>
+      <c r="H36">
+        <v>64</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>36</v>
+      </c>
+      <c r="H37">
+        <v>63</v>
+      </c>
+      <c r="I37">
+        <f>G37+H37</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>37</v>
+      </c>
+      <c r="H38">
+        <v>62</v>
+      </c>
+      <c r="I38">
+        <f>G38+H38</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>38</v>
+      </c>
+      <c r="H39">
+        <v>61</v>
+      </c>
+      <c r="I39">
+        <f t="shared" ref="I39:I46" si="4">G39+H39</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>39</v>
+      </c>
+      <c r="H40">
+        <v>60</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>40</v>
+      </c>
+      <c r="H41">
+        <v>59</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>41</v>
+      </c>
+      <c r="H42">
+        <v>58</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>42</v>
+      </c>
+      <c r="H43">
+        <v>57</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>43</v>
+      </c>
+      <c r="H44">
+        <v>56</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>44</v>
+      </c>
+      <c r="H45">
+        <v>55</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>45</v>
+      </c>
+      <c r="H46">
+        <v>54</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>46</v>
+      </c>
+      <c r="H47">
+        <v>53</v>
+      </c>
+      <c r="I47">
+        <f>G47+H47</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>47</v>
+      </c>
+      <c r="H48">
+        <v>52</v>
+      </c>
+      <c r="I48">
+        <f>G48+H48</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>48</v>
+      </c>
+      <c r="H49">
+        <v>51</v>
+      </c>
+      <c r="I49">
+        <f t="shared" ref="I49:I50" si="5">G49+H49</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>49</v>
+      </c>
+      <c r="H50">
+        <v>50</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="5"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>50</v>
+      </c>
+      <c r="H51">
+        <v>49</v>
+      </c>
+      <c r="I51">
+        <f t="shared" ref="I51:I90" si="6">G51+H51</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>51</v>
+      </c>
+      <c r="H52">
+        <v>48</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>52</v>
+      </c>
+      <c r="H53">
+        <v>47</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>53</v>
+      </c>
+      <c r="H54">
+        <v>46</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>54</v>
+      </c>
+      <c r="H55">
+        <v>45</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>55</v>
+      </c>
+      <c r="H56">
+        <v>44</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>56</v>
+      </c>
+      <c r="H57">
+        <v>43</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>57</v>
+      </c>
+      <c r="H58">
+        <v>42</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>58</v>
+      </c>
+      <c r="H59">
+        <v>41</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>59</v>
+      </c>
+      <c r="H60">
+        <v>40</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>60</v>
+      </c>
+      <c r="H61">
+        <v>39</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>61</v>
+      </c>
+      <c r="H62">
+        <v>38</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>62</v>
+      </c>
+      <c r="H63">
+        <v>37</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>63</v>
+      </c>
+      <c r="H64">
+        <v>36</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>64</v>
+      </c>
+      <c r="H65">
+        <v>35</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>65</v>
+      </c>
+      <c r="H66">
+        <v>34</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>66</v>
+      </c>
+      <c r="H67">
+        <v>33</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>67</v>
+      </c>
+      <c r="H68">
+        <v>32</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>68</v>
+      </c>
+      <c r="H69">
+        <v>31</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>69</v>
+      </c>
+      <c r="H70">
+        <v>30</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>70</v>
+      </c>
+      <c r="H71">
+        <v>29</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>71</v>
+      </c>
+      <c r="H72">
+        <v>28</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>72</v>
+      </c>
+      <c r="H73">
+        <v>27</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>73</v>
+      </c>
+      <c r="H74">
+        <v>26</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>74</v>
+      </c>
+      <c r="H75">
+        <v>25</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>75</v>
+      </c>
+      <c r="H76">
+        <v>24</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>76</v>
+      </c>
+      <c r="H77">
+        <v>23</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G78">
+        <v>77</v>
+      </c>
+      <c r="H78">
+        <v>22</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G79">
+        <v>78</v>
+      </c>
+      <c r="H79">
+        <v>21</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <v>79</v>
+      </c>
+      <c r="H80">
+        <v>20</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G81">
+        <v>80</v>
+      </c>
+      <c r="H81">
+        <v>19</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <v>81</v>
+      </c>
+      <c r="H82">
+        <v>18</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G83">
+        <v>82</v>
+      </c>
+      <c r="H83">
+        <v>17</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G84">
+        <v>83</v>
+      </c>
+      <c r="H84">
+        <v>16</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G85">
+        <v>84</v>
+      </c>
+      <c r="H85">
+        <v>15</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G86">
+        <v>85</v>
+      </c>
+      <c r="H86">
+        <v>14</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G87">
+        <v>86</v>
+      </c>
+      <c r="H87">
+        <v>13</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G88">
+        <v>87</v>
+      </c>
+      <c r="H88">
+        <v>12</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G89">
+        <v>88</v>
+      </c>
+      <c r="H89">
+        <v>11</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G90">
+        <v>89</v>
+      </c>
+      <c r="H90">
+        <v>10</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>